<commit_message>
PWR- Review of renewable capacity factors
Reviewed assumptions on renewables capacity factors
</commit_message>
<xml_diff>
--- a/SuppXls/Scen_00_DataByTimeslice_20.xlsx
+++ b/SuppXls/Scen_00_DataByTimeslice_20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Veda\Veda_models\Chiodi\TIMES-GEO\SuppXls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01137F7-4A5E-43D0-BE5B-3ED48DE32EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA6BF8C-91D0-4A30-848F-100B2ECCA68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4044" yWindow="1776" windowWidth="23040" windowHeight="12264" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11385" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="9" r:id="rId1"/>
@@ -49,8 +49,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Chiodi</author>
+  </authors>
+  <commentList>
+    <comment ref="F156" authorId="0" shapeId="0" xr:uid="{F8F8235B-97AD-443B-AC7A-E5D7205C1977}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Chiodi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="215">
   <si>
     <t>Residential</t>
   </si>
@@ -728,12 +762,6 @@
     </r>
   </si>
   <si>
-    <t>CSET_cn</t>
-  </si>
-  <si>
-    <t>ELCC, ELCD, HETC, HETD</t>
-  </si>
-  <si>
     <t>Original developer:</t>
   </si>
   <si>
@@ -766,6 +794,9 @@
   <si>
     <t>Base-year:</t>
   </si>
+  <si>
+    <t>ELCC, ELCD</t>
+  </si>
 </sst>
 </file>
 
@@ -781,9 +812,9 @@
     <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="170" formatCode="_ &quot;kr&quot;\ * #,##0_ ;_ &quot;kr&quot;\ * \-#,##0_ ;_ &quot;kr&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="171" formatCode="_ &quot;kr&quot;\ * #,##0.00_ ;_ &quot;kr&quot;\ * \-#,##0.00_ ;_ &quot;kr&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="0.0"/>
   </numFmts>
-  <fonts count="63" x14ac:knownFonts="1">
+  <fonts count="65" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1217,6 +1248,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="41">
@@ -4644,7 +4688,7 @@
     <xf numFmtId="0" fontId="39" fillId="31" borderId="0" xfId="621" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="36" fillId="31" borderId="0" xfId="621" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="36" fillId="31" borderId="0" xfId="621" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="621" applyAlignment="1">
@@ -6795,17 +6839,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" style="2" customWidth="1"/>
-    <col min="2" max="4" width="28.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.109375" style="2"/>
-    <col min="9" max="10" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="29.85546875" style="2" customWidth="1"/>
+    <col min="2" max="4" width="28.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="2"/>
+    <col min="9" max="10" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="109" t="s">
         <v>49</v>
       </c>
@@ -6813,42 +6857,42 @@
       <c r="C1" s="110"/>
       <c r="D1" s="111"/>
     </row>
-    <row r="2" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="91"/>
       <c r="B2" s="5"/>
       <c r="F2" s="93"/>
     </row>
-    <row r="3" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A3" s="91"/>
       <c r="B3" s="5"/>
       <c r="F3" s="93"/>
     </row>
-    <row r="4" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A4" s="91"/>
       <c r="B4" s="5"/>
       <c r="F4" s="93"/>
     </row>
-    <row r="5" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="91"/>
       <c r="B5" s="5"/>
       <c r="F5" s="93"/>
     </row>
-    <row r="6" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A6" s="91"/>
       <c r="B6" s="5"/>
       <c r="F6" s="93"/>
     </row>
-    <row r="7" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A7" s="91"/>
       <c r="B7" s="5"/>
       <c r="F7" s="93"/>
     </row>
-    <row r="8" spans="1:6" s="92" customFormat="1" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="92" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A8" s="91"/>
       <c r="B8" s="5"/>
       <c r="F8" s="93"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
@@ -6859,7 +6903,7 @@
       <c r="D9" s="14"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -6870,9 +6914,9 @@
       <c r="D10" s="14"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B11" s="16">
         <v>2018</v>
@@ -6881,26 +6925,26 @@
       <c r="D11" s="14"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="94" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="95"/>
       <c r="B13" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
@@ -6910,9 +6954,9 @@
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="96" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B15" s="97">
         <v>1</v>
@@ -6920,49 +6964,49 @@
       <c r="C15" s="18"/>
       <c r="D15" s="98"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="96" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B16" s="99" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="98"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="96" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="112" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C17" s="112"/>
       <c r="D17" s="112"/>
     </row>
-    <row r="18" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="98"/>
       <c r="B18" s="100" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C18" s="101"/>
       <c r="D18" s="101"/>
     </row>
-    <row r="19" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="98"/>
       <c r="B19" s="100"/>
       <c r="C19" s="101"/>
       <c r="D19" s="101"/>
     </row>
-    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>4</v>
       </c>
@@ -6970,7 +7014,7 @@
       <c r="C21" s="107"/>
       <c r="D21" s="108"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="102" t="s">
         <v>5</v>
       </c>
@@ -6980,7 +7024,7 @@
       <c r="C22" s="30"/>
       <c r="D22" s="31"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="103" t="s">
         <v>5</v>
       </c>
@@ -6990,7 +7034,7 @@
       <c r="C23" s="30"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="29" t="s">
         <v>50</v>
@@ -6998,13 +7042,13 @@
       <c r="C24" s="30"/>
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>8</v>
       </c>
@@ -7012,7 +7056,7 @@
       <c r="C26" s="107"/>
       <c r="D26" s="108"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="41" t="s">
         <v>9</v>
@@ -7020,7 +7064,7 @@
       <c r="C27" s="42"/>
       <c r="D27" s="43"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="41" t="s">
         <v>51</v>
@@ -7028,7 +7072,7 @@
       <c r="C28" s="42"/>
       <c r="D28" s="43"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
       <c r="B29" s="35" t="s">
         <v>52</v>
@@ -7036,13 +7080,13 @@
       <c r="C29" s="35"/>
       <c r="D29" s="34"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20"/>
       <c r="D30" s="14"/>
     </row>
-    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>10</v>
       </c>
@@ -7050,7 +7094,7 @@
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>11</v>
       </c>
@@ -7061,7 +7105,7 @@
       <c r="D32" s="9"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
         <v>19</v>
       </c>
@@ -7071,7 +7115,7 @@
       <c r="C33" s="38"/>
       <c r="D33" s="39"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
         <v>201</v>
       </c>
@@ -7081,7 +7125,7 @@
       <c r="C34" s="38"/>
       <c r="D34" s="39"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>18</v>
       </c>
@@ -7091,12 +7135,12 @@
       <c r="C35" s="105"/>
       <c r="D35" s="106"/>
     </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>14</v>
       </c>
@@ -7105,7 +7149,7 @@
         <v>4.1868000000000002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>15</v>
       </c>
@@ -7114,14 +7158,14 @@
         <v>3.6000000000000003E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D42" s="14"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>36</v>
       </c>
@@ -7134,7 +7178,7 @@
       <c r="D43" s="14"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>196</v>
       </c>
@@ -7147,7 +7191,7 @@
       <c r="D44" s="14"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>199</v>
       </c>
@@ -7160,16 +7204,16 @@
       <c r="D45" s="14"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D46" s="14"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="48" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="47" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="48" t="s">
         <v>54</v>
       </c>
@@ -7180,7 +7224,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="50" t="s">
         <v>56</v>
       </c>
@@ -7191,7 +7235,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="53" t="s">
         <v>59</v>
       </c>
@@ -7202,7 +7246,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="36" x14ac:dyDescent="0.25">
       <c r="A52" s="53" t="s">
         <v>62</v>
       </c>
@@ -7213,7 +7257,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="144" x14ac:dyDescent="0.25">
       <c r="A53" s="53" t="s">
         <v>65</v>
       </c>
@@ -7224,7 +7268,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="53" t="s">
         <v>68</v>
       </c>
@@ -7235,7 +7279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="53" t="s">
         <v>71</v>
       </c>
@@ -7246,7 +7290,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="48" x14ac:dyDescent="0.25">
       <c r="A56" s="61" t="s">
         <v>73</v>
       </c>
@@ -7257,7 +7301,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="36" x14ac:dyDescent="0.25">
       <c r="A57" s="53" t="s">
         <v>76</v>
       </c>
@@ -7268,7 +7312,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="53" t="s">
         <v>79</v>
       </c>
@@ -7279,7 +7323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="120" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="132" x14ac:dyDescent="0.25">
       <c r="A59" s="53" t="s">
         <v>82</v>
       </c>
@@ -7290,7 +7334,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="53" t="s">
         <v>41</v>
       </c>
@@ -7301,7 +7345,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="53" t="s">
         <v>85</v>
       </c>
@@ -7312,7 +7356,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="53" t="s">
         <v>87</v>
       </c>
@@ -7323,7 +7367,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A63" s="53" t="s">
         <v>90</v>
       </c>
@@ -7334,7 +7378,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="53" t="s">
         <v>93</v>
       </c>
@@ -7345,7 +7389,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="60" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="53" t="s">
         <v>96</v>
       </c>
@@ -7356,7 +7400,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="48" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="48" x14ac:dyDescent="0.25">
       <c r="A66" s="61" t="s">
         <v>99</v>
       </c>
@@ -7367,7 +7411,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="53" t="s">
         <v>102</v>
       </c>
@@ -7378,7 +7422,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="53" t="s">
         <v>105</v>
       </c>
@@ -7389,7 +7433,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="53" t="s">
         <v>47</v>
       </c>
@@ -7400,7 +7444,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="53" t="s">
         <v>108</v>
       </c>
@@ -7411,7 +7455,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="61" t="s">
         <v>110</v>
       </c>
@@ -7422,7 +7466,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="53" t="s">
         <v>112</v>
       </c>
@@ -7433,7 +7477,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="252" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="276" x14ac:dyDescent="0.25">
       <c r="A73" s="53" t="s">
         <v>115</v>
       </c>
@@ -7444,7 +7488,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="48" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="48" x14ac:dyDescent="0.25">
       <c r="A74" s="53" t="s">
         <v>118</v>
       </c>
@@ -7455,7 +7499,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="53" t="s">
         <v>121</v>
       </c>
@@ -7466,7 +7510,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="53" t="s">
         <v>123</v>
       </c>
@@ -7477,7 +7521,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="53" t="s">
         <v>125</v>
       </c>
@@ -7488,7 +7532,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="53" t="s">
         <v>127</v>
       </c>
@@ -7499,7 +7543,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="53" t="s">
         <v>129</v>
       </c>
@@ -7510,7 +7554,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="53" t="s">
         <v>131</v>
       </c>
@@ -7550,33 +7594,33 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" style="26" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="26" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9" style="26" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="18" width="9" style="26" customWidth="1"/>
-    <col min="19" max="16384" width="9.109375" style="26"/>
+    <col min="19" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B1" s="21" t="s">
         <v>133</v>
       </c>
       <c r="C1" s="69"/>
       <c r="D1" s="69"/>
     </row>
-    <row r="2" spans="2:14" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="21"/>
       <c r="C2" s="69"/>
       <c r="D2" s="69"/>
       <c r="G2" s="21"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>24</v>
       </c>
@@ -7585,7 +7629,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>20</v>
       </c>
@@ -7616,7 +7660,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>26</v>
       </c>
@@ -7645,7 +7689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="69" t="s">
         <v>25</v>
       </c>
@@ -7674,7 +7718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="69" t="s">
         <v>25</v>
       </c>
@@ -7703,7 +7747,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="69" t="s">
         <v>25</v>
       </c>
@@ -7732,7 +7776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="69" t="s">
         <v>25</v>
       </c>
@@ -7752,7 +7796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="69" t="s">
         <v>25</v>
       </c>
@@ -7772,7 +7816,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="69" t="s">
         <v>25</v>
       </c>
@@ -7783,7 +7827,7 @@
         <v>5.194063926940639E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
         <v>25</v>
       </c>
@@ -7794,7 +7838,7 @@
         <v>4.1552511415525115E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
         <v>25</v>
       </c>
@@ -7805,7 +7849,7 @@
         <v>5.194063926940639E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="69" t="s">
         <v>25</v>
       </c>
@@ -7816,7 +7860,7 @@
         <v>5.194063926940639E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="69" t="s">
         <v>25</v>
       </c>
@@ -7827,7 +7871,7 @@
         <v>5.194063926940639E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="69" t="s">
         <v>25</v>
       </c>
@@ -7838,7 +7882,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="69" t="s">
         <v>25</v>
       </c>
@@ -7849,7 +7893,7 @@
         <v>4.2009132420091327E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="69" t="s">
         <v>25</v>
       </c>
@@ -7860,7 +7904,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="69" t="s">
         <v>25</v>
       </c>
@@ -7871,7 +7915,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="69" t="s">
         <v>25</v>
       </c>
@@ -7882,7 +7926,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="69" t="s">
         <v>25</v>
       </c>
@@ -7893,7 +7937,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="69" t="s">
         <v>25</v>
       </c>
@@ -7904,7 +7948,7 @@
         <v>4.2009132420091327E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="69" t="s">
         <v>25</v>
       </c>
@@ -7915,7 +7959,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="69" t="s">
         <v>25</v>
       </c>
@@ -7926,7 +7970,7 @@
         <v>5.2511415525114152E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="78" t="s">
         <v>25</v>
       </c>
@@ -7943,34 +7987,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F348AB0B-58AE-45EC-B048-AE15E86A54C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F348AB0B-58AE-45EC-B048-AE15E86A54C4}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AJ175"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I133" sqref="I133"/>
+    <sheetView topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="26" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="26"/>
-    <col min="4" max="4" width="16.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="36" width="9.5546875" style="26" customWidth="1"/>
-    <col min="37" max="16384" width="9.109375" style="26"/>
+    <col min="2" max="2" width="9.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="26"/>
+    <col min="4" max="4" width="16.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="36" width="9.5703125" style="26" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>188</v>
       </c>
       <c r="B1" s="21"/>
     </row>
-    <row r="2" spans="1:36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -7978,11 +8022,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="70"/>
       <c r="B3" s="70"/>
     </row>
-    <row r="4" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="83" t="s">
         <v>175</v>
       </c>
@@ -8021,7 +8065,7 @@
       <c r="AI4" s="71"/>
       <c r="AJ4" s="71"/>
     </row>
-    <row r="5" spans="1:36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="83" t="s">
         <v>176</v>
       </c>
@@ -8030,7 +8074,7 @@
       </c>
       <c r="G5" s="82"/>
     </row>
-    <row r="6" spans="1:36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="83" t="s">
         <v>186</v>
       </c>
@@ -8039,13 +8083,13 @@
       </c>
       <c r="G6" s="82"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="22"/>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>20</v>
       </c>
@@ -8059,7 +8103,7 @@
         <v>171</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F9" s="24" t="str">
         <f>Legend!$A$50</f>
@@ -8186,7 +8230,7 @@
         <v>ZAF</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
@@ -8325,7 +8369,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="75" t="s">
         <v>44</v>
       </c>
@@ -8341,7 +8385,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E11" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F11" s="72">
         <v>0</v>
@@ -8437,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
         <v>44</v>
       </c>
@@ -8453,7 +8497,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E12" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F12" s="72">
         <v>8.5338686888358718E-4</v>
@@ -8549,7 +8593,7 @@
         <v>6.1644496195981428E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="75" t="s">
         <v>44</v>
       </c>
@@ -8565,7 +8609,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E13" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F13" s="72">
         <v>6.5962019617772982E-2</v>
@@ -8661,7 +8705,7 @@
         <v>6.8294753434607489E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="75" t="s">
         <v>44</v>
       </c>
@@ -8677,7 +8721,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E14" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F14" s="72">
         <v>0.18652475631443127</v>
@@ -8773,7 +8817,7 @@
         <v>0.19073984542125028</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
         <v>44</v>
       </c>
@@ -8789,7 +8833,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E15" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F15" s="72">
         <v>6.7114490669676506E-3</v>
@@ -8885,7 +8929,7 @@
         <v>7.1728066103536004E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
         <v>44</v>
       </c>
@@ -8901,7 +8945,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E16" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F16" s="72">
         <v>0</v>
@@ -8997,7 +9041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="75" t="s">
         <v>44</v>
       </c>
@@ -9013,7 +9057,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E17" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F17" s="72">
         <v>6.5900081942742975E-4</v>
@@ -9109,7 +9153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="75" t="s">
         <v>44</v>
       </c>
@@ -9125,7 +9169,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E18" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F18" s="72">
         <v>4.9563968492524771E-2</v>
@@ -9221,7 +9265,7 @@
         <v>3.4358248360807343E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
         <v>44</v>
       </c>
@@ -9237,7 +9281,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E19" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F19" s="72">
         <v>0.18555536241960718</v>
@@ -9333,7 +9377,7 @@
         <v>0.18984575239583815</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="75" t="s">
         <v>44</v>
       </c>
@@ -9349,7 +9393,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E20" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F20" s="72">
         <v>5.5272078531388843E-3</v>
@@ -9445,7 +9489,7 @@
         <v>1.160424937601149E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="75" t="s">
         <v>44</v>
       </c>
@@ -9461,7 +9505,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E21" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F21" s="72">
         <v>0</v>
@@ -9557,7 +9601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="75" t="s">
         <v>44</v>
       </c>
@@ -9573,7 +9617,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E22" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F22" s="72">
         <v>7.7846041780567268E-4</v>
@@ -9669,7 +9713,7 @@
         <v>1.8774132123323496E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="75" t="s">
         <v>44</v>
       </c>
@@ -9685,7 +9729,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E23" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F23" s="72">
         <v>6.1093878867984397E-2</v>
@@ -9781,7 +9825,7 @@
         <v>3.388496171608351E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="75" t="s">
         <v>44</v>
       </c>
@@ -9797,7 +9841,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E24" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F24" s="72">
         <v>0.18144379521052559</v>
@@ -9893,7 +9937,7 @@
         <v>0.19497850865283362</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="75" t="s">
         <v>44</v>
       </c>
@@ -9909,7 +9953,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E25" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F25" s="72">
         <v>6.1055719043582165E-3</v>
@@ -10005,7 +10049,7 @@
         <v>1.5089708694121259E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="75" t="s">
         <v>44</v>
       </c>
@@ -10021,7 +10065,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E26" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F26" s="72">
         <v>0</v>
@@ -10117,7 +10161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="75" t="s">
         <v>44</v>
       </c>
@@ -10133,7 +10177,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E27" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F27" s="72">
         <v>9.9502330700043467E-4</v>
@@ -10229,7 +10273,7 @@
         <v>8.348026654383824E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="75" t="s">
         <v>44</v>
       </c>
@@ -10245,7 +10289,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E28" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F28" s="72">
         <v>5.8385634999413787E-2</v>
@@ -10341,7 +10385,7 @@
         <v>6.5476107272709569E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="75" t="s">
         <v>44</v>
       </c>
@@ -10357,7 +10401,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E29" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F29" s="72">
         <v>0.18451911377341587</v>
@@ -10453,7 +10497,7 @@
         <v>0.2041181262459352</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="76" t="s">
         <v>44</v>
       </c>
@@ -10469,7 +10513,7 @@
         <v>P_SOL-PV</v>
       </c>
       <c r="E30" s="76" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F30" s="73">
         <v>5.3213700667422521E-3</v>
@@ -10565,7 +10609,7 @@
         <v>6.9914723230464536E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="83" t="s">
         <v>175</v>
       </c>
@@ -10604,7 +10648,7 @@
       <c r="AI33" s="71"/>
       <c r="AJ33" s="71"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="83" t="s">
         <v>176</v>
       </c>
@@ -10646,7 +10690,7 @@
       <c r="AI34"/>
       <c r="AJ34"/>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="83" t="s">
         <v>186</v>
       </c>
@@ -10688,13 +10732,13 @@
       <c r="AI35"/>
       <c r="AJ35"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B37" s="22"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>20</v>
       </c>
@@ -10708,7 +10752,7 @@
         <v>171</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F38" s="24" t="str">
         <f>Legend!$A$50</f>
@@ -10835,7 +10879,7 @@
         <v>ZAF</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:36" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>32</v>
       </c>
@@ -10974,7 +11018,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="75" t="s">
         <v>44</v>
       </c>
@@ -10990,7 +11034,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E40" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F40" s="72">
         <v>0</v>
@@ -11086,7 +11130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="75" t="s">
         <v>44</v>
       </c>
@@ -11102,7 +11146,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E41" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F41" s="72">
         <v>8.983949631337345E-4</v>
@@ -11198,7 +11242,7 @@
         <v>6.3905239592394433E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="75" t="s">
         <v>44</v>
       </c>
@@ -11214,7 +11258,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E42" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F42" s="72">
         <v>6.4938877877145765E-2</v>
@@ -11310,7 +11354,7 @@
         <v>6.9450886487931823E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="75" t="s">
         <v>44</v>
       </c>
@@ -11326,7 +11370,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E43" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F43" s="72">
         <v>0.18767945845653694</v>
@@ -11422,7 +11466,7 @@
         <v>0.18949124711989193</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="75" t="s">
         <v>44</v>
       </c>
@@ -11438,7 +11482,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E44" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F44" s="72">
         <v>6.6358718867832647E-3</v>
@@ -11534,7 +11578,7 @@
         <v>7.3300139750652948E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="75" t="s">
         <v>44</v>
       </c>
@@ -11550,7 +11594,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E45" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F45" s="72">
         <v>0</v>
@@ -11646,7 +11690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="75" t="s">
         <v>44</v>
       </c>
@@ -11662,7 +11706,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E46" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F46" s="72">
         <v>6.6454102970192358E-4</v>
@@ -11758,7 +11802,7 @@
         <v>4.9156295982054157E-6</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="75" t="s">
         <v>44</v>
       </c>
@@ -11774,7 +11818,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E47" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F47" s="72">
         <v>4.996827334707718E-2</v>
@@ -11870,7 +11914,7 @@
         <v>3.4927514547088749E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="75" t="s">
         <v>44</v>
       </c>
@@ -11886,7 +11930,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E48" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F48" s="72">
         <v>0.18489902203495862</v>
@@ -11982,7 +12026,7 @@
         <v>0.18918668396938479</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="75" t="s">
         <v>44</v>
       </c>
@@ -11998,7 +12042,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E49" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F49" s="72">
         <v>5.505266373511032E-3</v>
@@ -12094,7 +12138,7 @@
         <v>1.1728692221318123E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="75" t="s">
         <v>44</v>
       </c>
@@ -12110,7 +12154,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E50" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F50" s="72">
         <v>0</v>
@@ -12206,7 +12250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="75" t="s">
         <v>44</v>
       </c>
@@ -12222,7 +12266,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E51" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F51" s="72">
         <v>8.0827099109228207E-4</v>
@@ -12318,7 +12362,7 @@
         <v>2.4441227311338269E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="75" t="s">
         <v>44</v>
       </c>
@@ -12334,7 +12378,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E52" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F52" s="72">
         <v>6.057794308145191E-2</v>
@@ -12430,7 +12474,7 @@
         <v>3.3946984641040304E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="75" t="s">
         <v>44</v>
       </c>
@@ -12446,7 +12490,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E53" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F53" s="72">
         <v>0.18201164575101189</v>
@@ -12542,7 +12586,7 @@
         <v>0.19492041632458487</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="75" t="s">
         <v>44</v>
       </c>
@@ -12558,7 +12602,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E54" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F54" s="72">
         <v>5.9939197092236662E-3</v>
@@ -12654,7 +12698,7 @@
         <v>1.4956151020130452E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="75" t="s">
         <v>44</v>
       </c>
@@ -12670,7 +12714,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E55" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F55" s="72">
         <v>0</v>
@@ -12766,7 +12810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="75" t="s">
         <v>44</v>
       </c>
@@ -12782,7 +12826,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E56" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F56" s="72">
         <v>1.0162568879134362E-3</v>
@@ -12878,7 +12922,7 @@
         <v>8.8920917691304451E-4</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="75" t="s">
         <v>44</v>
       </c>
@@ -12894,7 +12938,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E57" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F57" s="72">
         <v>5.7381963319941588E-2</v>
@@ -12990,7 +13034,7 @@
         <v>6.7094040884810052E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="75" t="s">
         <v>44</v>
       </c>
@@ -13006,7 +13050,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E58" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F58" s="72">
         <v>0.1857010710027216</v>
@@ -13102,7 +13146,7 @@
         <v>0.20222993193675676</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="76" t="s">
         <v>44</v>
       </c>
@@ -13118,7 +13162,7 @@
         <v>P_SOL-CSP</v>
       </c>
       <c r="E59" s="76" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F59" s="73">
         <v>5.3192232877951502E-3</v>
@@ -13214,7 +13258,7 @@
         <v>7.19617735955402E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A62" s="83" t="s">
         <v>175</v>
       </c>
@@ -13253,7 +13297,7 @@
       <c r="AI62" s="71"/>
       <c r="AJ62" s="71"/>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="83" t="s">
         <v>176</v>
       </c>
@@ -13295,7 +13339,7 @@
       <c r="AI63"/>
       <c r="AJ63"/>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="83" t="s">
         <v>186</v>
       </c>
@@ -13337,13 +13381,13 @@
       <c r="AI64"/>
       <c r="AJ64"/>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B66" s="22"/>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
         <v>20</v>
       </c>
@@ -13357,7 +13401,7 @@
         <v>171</v>
       </c>
       <c r="E67" s="24" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F67" s="24" t="str">
         <f>Legend!$A$50</f>
@@ -13484,7 +13528,7 @@
         <v>ZAF</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:36" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>32</v>
       </c>
@@ -13623,7 +13667,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="75" t="s">
         <v>44</v>
       </c>
@@ -13639,7 +13683,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E69" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F69" s="72">
         <v>5.1790239785315974E-2</v>
@@ -13735,7 +13779,7 @@
         <v>1.9364803790644817E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="75" t="s">
         <v>44</v>
       </c>
@@ -13751,7 +13795,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E70" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F70" s="72">
         <v>3.6215024465263916E-2</v>
@@ -13847,7 +13891,7 @@
         <v>1.2528478927096357E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="75" t="s">
         <v>44</v>
       </c>
@@ -13863,7 +13907,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E71" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F71" s="72">
         <v>4.7965305955017495E-2</v>
@@ -13959,7 +14003,7 @@
         <v>1.5077033284288222E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="75" t="s">
         <v>44</v>
       </c>
@@ -13975,7 +14019,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E72" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F72" s="72">
         <v>4.4696629814720841E-2</v>
@@ -14071,7 +14115,7 @@
         <v>0.15203482901962129</v>
       </c>
     </row>
-    <row r="73" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="75" t="s">
         <v>44</v>
       </c>
@@ -14087,7 +14131,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E73" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F73" s="72">
         <v>0.10571831307859345</v>
@@ -14183,7 +14227,7 @@
         <v>3.03300928454996E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="75" t="s">
         <v>44</v>
       </c>
@@ -14199,7 +14243,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E74" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F74" s="72">
         <v>3.2180138219639873E-2</v>
@@ -14295,7 +14339,7 @@
         <v>1.9740531597421413E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="75" t="s">
         <v>44</v>
       </c>
@@ -14311,7 +14355,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E75" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F75" s="72">
         <v>2.577893458973287E-2</v>
@@ -14407,7 +14451,7 @@
         <v>1.6826812965842607E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="75" t="s">
         <v>44</v>
       </c>
@@ -14423,7 +14467,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E76" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F76" s="72">
         <v>9.5336965217722572E-2</v>
@@ -14519,7 +14563,7 @@
         <v>1.8744103090723475E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="75" t="s">
         <v>44</v>
       </c>
@@ -14535,7 +14579,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E77" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F77" s="72">
         <v>3.1735673830161723E-2</v>
@@ -14631,7 +14675,7 @@
         <v>0.15956172913423541</v>
       </c>
     </row>
-    <row r="78" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="75" t="s">
         <v>44</v>
       </c>
@@ -14647,7 +14691,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E78" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F78" s="72">
         <v>3.5827495477625544E-2</v>
@@ -14743,7 +14787,7 @@
         <v>2.0761563277124237E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="75" t="s">
         <v>44</v>
       </c>
@@ -14759,7 +14803,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E79" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F79" s="72">
         <v>4.1738021436334594E-2</v>
@@ -14855,7 +14899,7 @@
         <v>3.405688137813731E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="75" t="s">
         <v>44</v>
       </c>
@@ -14871,7 +14915,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E80" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F80" s="72">
         <v>3.5744094310223906E-2</v>
@@ -14967,7 +15011,7 @@
         <v>2.7961977741032013E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="75" t="s">
         <v>44</v>
       </c>
@@ -14983,7 +15027,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E81" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F81" s="72">
         <v>0.10514686273762808</v>
@@ -15079,7 +15123,7 @@
         <v>3.2223266908409001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="75" t="s">
         <v>44</v>
       </c>
@@ -15095,7 +15139,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E82" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F82" s="72">
         <v>3.2866619123563777E-2</v>
@@ -15191,7 +15235,7 @@
         <v>0.14557709085310572</v>
       </c>
     </row>
-    <row r="83" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="75" t="s">
         <v>44</v>
       </c>
@@ -15207,7 +15251,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E83" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F83" s="72">
         <v>3.9987150941400713E-2</v>
@@ -15303,7 +15347,7 @@
         <v>3.6178525049281568E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="75" t="s">
         <v>44</v>
       </c>
@@ -15319,7 +15363,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E84" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F84" s="72">
         <v>4.0881085440141136E-2</v>
@@ -15415,7 +15459,7 @@
         <v>2.5888242147025491E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="75" t="s">
         <v>44</v>
       </c>
@@ -15431,7 +15475,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E85" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F85" s="72">
         <v>2.941293570158876E-2</v>
@@ -15527,7 +15571,7 @@
         <v>1.7223513996118572E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="75" t="s">
         <v>44</v>
       </c>
@@ -15543,7 +15587,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E86" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F86" s="72">
         <v>4.217855726656923E-2</v>
@@ -15639,7 +15683,7 @@
         <v>2.0593380953872437E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="75" t="s">
         <v>44</v>
       </c>
@@ -15655,7 +15699,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E87" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F87" s="72">
         <v>4.0098313181221722E-2</v>
@@ -15751,7 +15795,7 @@
         <v>3.4011988311403361E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="76" t="s">
         <v>44</v>
       </c>
@@ -15767,7 +15811,7 @@
         <v>P_WIN-ON</v>
       </c>
       <c r="E88" s="76" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F88" s="73">
         <v>8.4701639427533712E-2</v>
@@ -15863,7 +15907,7 @@
         <v>0.16131515472911714</v>
       </c>
     </row>
-    <row r="91" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A91" s="83" t="s">
         <v>175</v>
       </c>
@@ -15902,7 +15946,7 @@
       <c r="AI91" s="71"/>
       <c r="AJ91" s="71"/>
     </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A92" s="83" t="s">
         <v>176</v>
       </c>
@@ -15944,7 +15988,7 @@
       <c r="AI92"/>
       <c r="AJ92"/>
     </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A93" s="83" t="s">
         <v>186</v>
       </c>
@@ -15986,13 +16030,13 @@
       <c r="AI93"/>
       <c r="AJ93"/>
     </row>
-    <row r="95" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A95" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B95" s="22"/>
     </row>
-    <row r="96" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A96" s="24" t="s">
         <v>20</v>
       </c>
@@ -16006,7 +16050,7 @@
         <v>171</v>
       </c>
       <c r="E96" s="24" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F96" s="24" t="str">
         <f>Legend!$A$50</f>
@@ -16133,7 +16177,7 @@
         <v>ZAF</v>
       </c>
     </row>
-    <row r="97" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:36" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A97" s="27" t="s">
         <v>32</v>
       </c>
@@ -16272,7 +16316,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="98" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="75" t="s">
         <v>44</v>
       </c>
@@ -16288,7 +16332,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E98" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F98" s="72">
         <v>4.8194350765051644E-2</v>
@@ -16385,7 +16429,7 @@
         <v>3.9566366835066508E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="75" t="s">
         <v>44</v>
       </c>
@@ -16401,7 +16445,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E99" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F99" s="72">
         <v>3.4829104569726849E-2</v>
@@ -16498,7 +16542,7 @@
         <v>2.7868821280303817E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="75" t="s">
         <v>44</v>
       </c>
@@ -16514,7 +16558,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E100" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F100" s="72">
         <v>9.0066972877267712E-2</v>
@@ -16611,7 +16655,7 @@
         <v>3.2555586221119336E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="75" t="s">
         <v>44</v>
       </c>
@@ -16627,7 +16671,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E101" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F101" s="72">
         <v>4.3988651851595548E-2</v>
@@ -16724,7 +16768,7 @@
         <v>0.10719982984153995</v>
       </c>
     </row>
-    <row r="102" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="75" t="s">
         <v>44</v>
       </c>
@@ -16740,7 +16784,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E102" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F102" s="72">
         <v>5.2264791019984526E-2</v>
@@ -16837,7 +16881,7 @@
         <v>4.8617116762095902E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="75" t="s">
         <v>44</v>
       </c>
@@ -16853,7 +16897,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E103" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F103" s="72">
         <v>3.1577290110205311E-2</v>
@@ -16950,7 +16994,7 @@
         <v>0.11226204402850153</v>
       </c>
     </row>
-    <row r="104" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="75" t="s">
         <v>44</v>
       </c>
@@ -16966,7 +17010,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E104" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F104" s="72">
         <v>2.5302595763732984E-2</v>
@@ -17063,7 +17107,7 @@
         <v>2.4743114782310394E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="75" t="s">
         <v>44</v>
       </c>
@@ -17079,7 +17123,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E105" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F105" s="72">
         <v>9.8072926021913726E-2</v>
@@ -17176,7 +17220,7 @@
         <v>2.7893241547237761E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="75" t="s">
         <v>44</v>
       </c>
@@ -17192,7 +17236,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E106" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F106" s="72">
         <v>3.5791962994900763E-2</v>
@@ -17289,7 +17333,7 @@
         <v>2.8748354767139234E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="75" t="s">
         <v>44</v>
       </c>
@@ -17305,7 +17349,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E107" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F107" s="72">
         <v>3.5864755272702067E-2</v>
@@ -17402,7 +17446,7 @@
         <v>3.4629326976268068E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="75" t="s">
         <v>44</v>
       </c>
@@ -17418,7 +17462,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E108" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F108" s="72">
         <v>4.6948767174903969E-2</v>
@@ -17515,7 +17559,7 @@
         <v>3.6641818990881557E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="75" t="s">
         <v>44</v>
       </c>
@@ -17531,7 +17575,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E109" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F109" s="72">
         <v>3.9706692985791728E-2</v>
@@ -17628,7 +17672,7 @@
         <v>2.8415511084746815E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="75" t="s">
         <v>44</v>
       </c>
@@ -17644,7 +17688,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E110" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F110" s="72">
         <v>5.0965452028010165E-2</v>
@@ -17741,7 +17785,7 @@
         <v>0.11349569286397956</v>
       </c>
     </row>
-    <row r="111" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="75" t="s">
         <v>44</v>
       </c>
@@ -17757,7 +17801,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E111" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F111" s="72">
         <v>4.9425866184956604E-2</v>
@@ -17854,7 +17898,7 @@
         <v>3.5789818914353642E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="75" t="s">
         <v>44</v>
       </c>
@@ -17870,7 +17914,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E112" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F112" s="72">
         <v>9.9150650483692995E-2</v>
@@ -17967,7 +18011,7 @@
         <v>3.9988754445091916E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="75" t="s">
         <v>44</v>
       </c>
@@ -17983,7 +18027,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E113" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F113" s="72">
         <v>3.1027465134843994E-2</v>
@@ -18080,7 +18124,7 @@
         <v>4.0996785203918258E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="75" t="s">
         <v>44</v>
       </c>
@@ -18096,7 +18140,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E114" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F114" s="72">
         <v>2.3200145933024816E-2</v>
@@ -18193,7 +18237,7 @@
         <v>2.9612085405370771E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="75" t="s">
         <v>44</v>
       </c>
@@ -18209,7 +18253,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E115" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F115" s="72">
         <v>9.6789920710271746E-2</v>
@@ -18306,7 +18350,7 @@
         <v>3.4111250207054994E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="75" t="s">
         <v>44</v>
       </c>
@@ -18322,7 +18366,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E116" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F116" s="72">
         <v>3.1302231515465913E-2</v>
@@ -18419,7 +18463,7 @@
         <v>4.7282431560556948E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="76" t="s">
         <v>44</v>
       </c>
@@ -18435,7 +18479,7 @@
         <v>P_WIN-OF</v>
       </c>
       <c r="E117" s="76" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F117" s="73">
         <v>3.5529406601956921E-2</v>
@@ -18532,7 +18576,7 @@
         <v>0.10958204828246305</v>
       </c>
     </row>
-    <row r="120" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A120" s="83" t="s">
         <v>175</v>
       </c>
@@ -18571,7 +18615,7 @@
       <c r="AI120" s="71"/>
       <c r="AJ120" s="71"/>
     </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A121" s="83" t="s">
         <v>176</v>
       </c>
@@ -18613,7 +18657,7 @@
       <c r="AI121"/>
       <c r="AJ121"/>
     </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A122" s="83" t="s">
         <v>186</v>
       </c>
@@ -18655,13 +18699,13 @@
       <c r="AI122"/>
       <c r="AJ122"/>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A124" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B124" s="22"/>
     </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A125" s="24" t="s">
         <v>20</v>
       </c>
@@ -18675,7 +18719,7 @@
         <v>171</v>
       </c>
       <c r="E125" s="24" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F125" s="24" t="str">
         <f>Legend!$A$50</f>
@@ -18802,7 +18846,7 @@
         <v>ZAF</v>
       </c>
     </row>
-    <row r="126" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:36" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A126" s="27" t="s">
         <v>32</v>
       </c>
@@ -18941,7 +18985,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="127" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="75" t="s">
         <v>44</v>
       </c>
@@ -18957,7 +19001,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E127" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F127" s="72">
         <v>4.1555187579399619E-2</v>
@@ -19053,7 +19097,7 @@
         <v>9.3271683673469399E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="75" t="s">
         <v>44</v>
       </c>
@@ -19069,7 +19113,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E128" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F128" s="72">
         <v>3.8562771622696938E-2</v>
@@ -19165,7 +19209,7 @@
         <v>6.8327717334811675E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="75" t="s">
         <v>44</v>
       </c>
@@ -19181,7 +19225,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E129" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F129" s="72">
         <v>4.1592456805928227E-2</v>
@@ -19277,7 +19321,7 @@
         <v>8.5409646668514597E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="75" t="s">
         <v>44</v>
       </c>
@@ -19293,7 +19337,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E130" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F130" s="72">
         <v>4.1592456805928227E-2</v>
@@ -19389,7 +19433,7 @@
         <v>8.5409646668514597E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="75" t="s">
         <v>44</v>
       </c>
@@ -19405,7 +19449,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E131" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F131" s="72">
         <v>4.1592456805928227E-2</v>
@@ -19501,7 +19545,7 @@
         <v>8.5409646668514597E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="75" t="s">
         <v>44</v>
       </c>
@@ -19517,7 +19561,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E132" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F132" s="72">
         <v>5.6473348385949626E-2</v>
@@ -19613,7 +19657,7 @@
         <v>8.5181451612903233E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="75" t="s">
         <v>44</v>
       </c>
@@ -19629,7 +19673,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E133" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F133" s="72">
         <v>4.8924731182795701E-2</v>
@@ -19725,7 +19769,7 @@
         <v>1.1456665858193875E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="75" t="s">
         <v>44</v>
       </c>
@@ -19741,7 +19785,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E134" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F134" s="72">
         <v>5.6554122015168178E-2</v>
@@ -19837,7 +19881,7 @@
         <v>1.4320832322742338E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="75" t="s">
         <v>44</v>
       </c>
@@ -19853,7 +19897,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E135" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F135" s="72">
         <v>5.6554122015168178E-2</v>
@@ -19949,7 +19993,7 @@
         <v>1.4320832322742338E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="75" t="s">
         <v>44</v>
       </c>
@@ -19965,7 +20009,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E136" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F136" s="72">
         <v>5.6554122015168178E-2</v>
@@ -20061,7 +20105,7 @@
         <v>1.4320832322742338E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="75" t="s">
         <v>44</v>
       </c>
@@ -20077,7 +20121,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E137" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F137" s="72">
         <v>5.9015984694875602E-2</v>
@@ -20173,7 +20217,7 @@
         <v>3.1944444444444456E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="75" t="s">
         <v>44</v>
       </c>
@@ -20189,7 +20233,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E138" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F138" s="72">
         <v>5.0432215897111526E-2</v>
@@ -20285,7 +20329,7 @@
         <v>1.3558897243107769E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="75" t="s">
         <v>44</v>
       </c>
@@ -20301,7 +20345,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E139" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F139" s="72">
         <v>5.9023802417050041E-2</v>
@@ -20397,7 +20441,7 @@
         <v>1.6948621553884713E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="75" t="s">
         <v>44</v>
       </c>
@@ -20413,7 +20457,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E140" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F140" s="72">
         <v>5.9023802417050041E-2</v>
@@ -20509,7 +20553,7 @@
         <v>1.6948621553884713E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="75" t="s">
         <v>44</v>
       </c>
@@ -20525,7 +20569,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E141" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F141" s="72">
         <v>5.9023802417050041E-2</v>
@@ -20621,7 +20665,7 @@
         <v>1.6948621553884713E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="75" t="s">
         <v>44</v>
       </c>
@@ -20637,7 +20681,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E142" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F142" s="72">
         <v>6.3040269871389415E-2</v>
@@ -20733,7 +20777,7 @@
         <v>8.442460317460318E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="75" t="s">
         <v>44</v>
       </c>
@@ -20749,7 +20793,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E143" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F143" s="72">
         <v>3.5891441484493108E-2</v>
@@ -20845,7 +20889,7 @@
         <v>5.5115207373271899E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="75" t="s">
         <v>44</v>
       </c>
@@ -20861,7 +20905,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E144" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F144" s="72">
         <v>4.4864301855616379E-2</v>
@@ -20957,7 +21001,7 @@
         <v>6.8894009216589863E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="75" t="s">
         <v>44</v>
       </c>
@@ -20973,7 +21017,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E145" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F145" s="72">
         <v>4.4864301855616379E-2</v>
@@ -21069,7 +21113,7 @@
         <v>6.8894009216589863E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="76" t="s">
         <v>44</v>
       </c>
@@ -21085,7 +21129,7 @@
         <v>P_HYD</v>
       </c>
       <c r="E146" s="76" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F146" s="73">
         <v>4.4864301855616379E-2</v>
@@ -21181,7 +21225,7 @@
         <v>6.8894009216589863E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:36" ht="18" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:36" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A149" s="83" t="s">
         <v>175</v>
       </c>
@@ -21220,7 +21264,7 @@
       <c r="AI149" s="71"/>
       <c r="AJ149" s="71"/>
     </row>
-    <row r="150" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A150" s="83" t="s">
         <v>176</v>
       </c>
@@ -21262,7 +21306,7 @@
       <c r="AI150"/>
       <c r="AJ150"/>
     </row>
-    <row r="151" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A151" s="83" t="s">
         <v>186</v>
       </c>
@@ -21304,13 +21348,13 @@
       <c r="AI151"/>
       <c r="AJ151"/>
     </row>
-    <row r="153" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A153" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B153" s="22"/>
     </row>
-    <row r="154" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A154" s="24" t="s">
         <v>20</v>
       </c>
@@ -21324,7 +21368,7 @@
         <v>171</v>
       </c>
       <c r="E154" s="24" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="F154" s="24" t="str">
         <f>Legend!$A$50</f>
@@ -21451,7 +21495,7 @@
         <v>ZAF</v>
       </c>
     </row>
-    <row r="155" spans="1:36" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:36" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A155" s="27" t="s">
         <v>32</v>
       </c>
@@ -21590,7 +21634,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="156" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="75" t="s">
         <v>44</v>
       </c>
@@ -21606,7 +21650,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E156" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F156" s="84">
         <f>F98</f>
@@ -21733,7 +21777,7 @@
         <v>3.9566366835066508E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A157" s="75" t="s">
         <v>44</v>
       </c>
@@ -21749,7 +21793,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E157" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F157" s="84">
         <f t="shared" ref="F157:AJ165" si="2">F99</f>
@@ -21876,7 +21920,7 @@
         <v>2.7868821280303817E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="75" t="s">
         <v>44</v>
       </c>
@@ -21892,7 +21936,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E158" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F158" s="84">
         <f t="shared" si="2"/>
@@ -22019,7 +22063,7 @@
         <v>3.2555586221119336E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="75" t="s">
         <v>44</v>
       </c>
@@ -22035,7 +22079,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E159" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F159" s="84">
         <f t="shared" si="2"/>
@@ -22162,7 +22206,7 @@
         <v>0.10719982984153995</v>
       </c>
     </row>
-    <row r="160" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="75" t="s">
         <v>44</v>
       </c>
@@ -22178,7 +22222,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E160" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F160" s="84">
         <f t="shared" si="2"/>
@@ -22305,7 +22349,7 @@
         <v>4.8617116762095902E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="75" t="s">
         <v>44</v>
       </c>
@@ -22321,7 +22365,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E161" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F161" s="84">
         <f t="shared" si="2"/>
@@ -22448,7 +22492,7 @@
         <v>0.11226204402850153</v>
       </c>
     </row>
-    <row r="162" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="75" t="s">
         <v>44</v>
       </c>
@@ -22464,7 +22508,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E162" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F162" s="84">
         <f t="shared" si="2"/>
@@ -22591,7 +22635,7 @@
         <v>2.4743114782310394E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="75" t="s">
         <v>44</v>
       </c>
@@ -22607,7 +22651,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E163" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F163" s="84">
         <f t="shared" si="2"/>
@@ -22734,7 +22778,7 @@
         <v>2.7893241547237761E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="75" t="s">
         <v>44</v>
       </c>
@@ -22750,7 +22794,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E164" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F164" s="84">
         <f t="shared" si="2"/>
@@ -22877,7 +22921,7 @@
         <v>2.8748354767139234E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="75" t="s">
         <v>44</v>
       </c>
@@ -22893,7 +22937,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E165" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F165" s="84">
         <f t="shared" si="2"/>
@@ -23020,7 +23064,7 @@
         <v>3.4629326976268068E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="75" t="s">
         <v>44</v>
       </c>
@@ -23036,7 +23080,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E166" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F166" s="84">
         <f t="shared" ref="F166:AJ174" si="4">F108</f>
@@ -23163,7 +23207,7 @@
         <v>3.6641818990881557E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="75" t="s">
         <v>44</v>
       </c>
@@ -23179,7 +23223,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E167" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F167" s="84">
         <f t="shared" si="4"/>
@@ -23306,7 +23350,7 @@
         <v>2.8415511084746815E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="75" t="s">
         <v>44</v>
       </c>
@@ -23322,7 +23366,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E168" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F168" s="84">
         <f t="shared" si="4"/>
@@ -23449,7 +23493,7 @@
         <v>0.11349569286397956</v>
       </c>
     </row>
-    <row r="169" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="75" t="s">
         <v>44</v>
       </c>
@@ -23465,7 +23509,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E169" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F169" s="84">
         <f t="shared" si="4"/>
@@ -23592,7 +23636,7 @@
         <v>3.5789818914353642E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="75" t="s">
         <v>44</v>
       </c>
@@ -23608,7 +23652,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E170" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F170" s="84">
         <f t="shared" si="4"/>
@@ -23735,7 +23779,7 @@
         <v>3.9988754445091916E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="75" t="s">
         <v>44</v>
       </c>
@@ -23751,7 +23795,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E171" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F171" s="84">
         <f t="shared" si="4"/>
@@ -23878,7 +23922,7 @@
         <v>4.0996785203918258E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A172" s="75" t="s">
         <v>44</v>
       </c>
@@ -23894,7 +23938,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E172" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F172" s="84">
         <f t="shared" si="4"/>
@@ -24021,7 +24065,7 @@
         <v>2.9612085405370771E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="75" t="s">
         <v>44</v>
       </c>
@@ -24037,7 +24081,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E173" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F173" s="84">
         <f t="shared" si="4"/>
@@ -24164,7 +24208,7 @@
         <v>3.4111250207054994E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="75" t="s">
         <v>44</v>
       </c>
@@ -24180,7 +24224,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E174" s="75" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F174" s="84">
         <f t="shared" si="4"/>
@@ -24307,7 +24351,7 @@
         <v>4.7282431560556948E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="76" t="s">
         <v>44</v>
       </c>
@@ -24323,7 +24367,7 @@
         <v>P_OCE</v>
       </c>
       <c r="E175" s="76" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F175" s="85">
         <f t="shared" ref="F175:AJ175" si="6">F117</f>
@@ -24453,6 +24497,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -24467,34 +24512,34 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="26" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="26" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" style="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="26"/>
+    <col min="2" max="2" width="11.28515625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="70"/>
     </row>
-    <row r="3" spans="1:35" s="74" customFormat="1" ht="21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" s="74" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
         <v>20</v>
       </c>
@@ -24601,7 +24646,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
         <v>32</v>
       </c>
@@ -24708,7 +24753,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="75" t="s">
         <v>21</v>
       </c>
@@ -24754,7 +24799,7 @@
       <c r="AH8" s="81"/>
       <c r="AI8" s="81"/>
     </row>
-    <row r="9" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="75" t="s">
         <v>21</v>
       </c>
@@ -24800,7 +24845,7 @@
       <c r="AH9" s="81"/>
       <c r="AI9" s="81"/>
     </row>
-    <row r="10" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="75" t="s">
         <v>21</v>
       </c>
@@ -24846,7 +24891,7 @@
       <c r="AH10" s="81"/>
       <c r="AI10" s="81"/>
     </row>
-    <row r="11" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="75" t="s">
         <v>21</v>
       </c>
@@ -24892,7 +24937,7 @@
       <c r="AH11" s="81"/>
       <c r="AI11" s="81"/>
     </row>
-    <row r="12" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
         <v>21</v>
       </c>
@@ -24938,7 +24983,7 @@
       <c r="AH12" s="81"/>
       <c r="AI12" s="81"/>
     </row>
-    <row r="13" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="75" t="s">
         <v>21</v>
       </c>
@@ -24984,7 +25029,7 @@
       <c r="AH13" s="81"/>
       <c r="AI13" s="81"/>
     </row>
-    <row r="14" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="75" t="s">
         <v>21</v>
       </c>
@@ -25030,7 +25075,7 @@
       <c r="AH14" s="81"/>
       <c r="AI14" s="81"/>
     </row>
-    <row r="15" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="75" t="s">
         <v>21</v>
       </c>
@@ -25076,7 +25121,7 @@
       <c r="AH15" s="81"/>
       <c r="AI15" s="81"/>
     </row>
-    <row r="16" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="75" t="s">
         <v>21</v>
       </c>
@@ -25122,7 +25167,7 @@
       <c r="AH16" s="81"/>
       <c r="AI16" s="81"/>
     </row>
-    <row r="17" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="75" t="s">
         <v>21</v>
       </c>
@@ -25168,7 +25213,7 @@
       <c r="AH17" s="81"/>
       <c r="AI17" s="81"/>
     </row>
-    <row r="18" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="75" t="s">
         <v>21</v>
       </c>
@@ -25214,7 +25259,7 @@
       <c r="AH18" s="81"/>
       <c r="AI18" s="81"/>
     </row>
-    <row r="19" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
         <v>21</v>
       </c>
@@ -25260,7 +25305,7 @@
       <c r="AH19" s="81"/>
       <c r="AI19" s="81"/>
     </row>
-    <row r="20" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="75" t="s">
         <v>21</v>
       </c>
@@ -25306,7 +25351,7 @@
       <c r="AH20" s="81"/>
       <c r="AI20" s="81"/>
     </row>
-    <row r="21" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="75" t="s">
         <v>21</v>
       </c>
@@ -25352,7 +25397,7 @@
       <c r="AH21" s="81"/>
       <c r="AI21" s="81"/>
     </row>
-    <row r="22" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="75" t="s">
         <v>21</v>
       </c>
@@ -25398,7 +25443,7 @@
       <c r="AH22" s="81"/>
       <c r="AI22" s="81"/>
     </row>
-    <row r="23" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="75" t="s">
         <v>21</v>
       </c>
@@ -25444,7 +25489,7 @@
       <c r="AH23" s="81"/>
       <c r="AI23" s="81"/>
     </row>
-    <row r="24" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="75" t="s">
         <v>21</v>
       </c>
@@ -25490,7 +25535,7 @@
       <c r="AH24" s="81"/>
       <c r="AI24" s="81"/>
     </row>
-    <row r="25" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="75" t="s">
         <v>21</v>
       </c>
@@ -25536,7 +25581,7 @@
       <c r="AH25" s="81"/>
       <c r="AI25" s="81"/>
     </row>
-    <row r="26" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="75" t="s">
         <v>21</v>
       </c>
@@ -25582,7 +25627,7 @@
       <c r="AH26" s="81"/>
       <c r="AI26" s="81"/>
     </row>
-    <row r="27" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="76" t="s">
         <v>21</v>
       </c>
@@ -25628,55 +25673,55 @@
       <c r="AH27" s="88"/>
       <c r="AI27" s="88"/>
     </row>
-    <row r="28" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="75"/>
       <c r="B28" s="75"/>
     </row>
-    <row r="29" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="75"/>
       <c r="B29" s="75"/>
     </row>
-    <row r="30" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="75"/>
       <c r="B30" s="75"/>
     </row>
-    <row r="31" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="75"/>
       <c r="B31" s="75"/>
     </row>
-    <row r="32" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="75"/>
       <c r="B32" s="75"/>
     </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="75"/>
       <c r="B33" s="75"/>
     </row>
-    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="75"/>
     </row>
-    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="75"/>
     </row>
-    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="75"/>
     </row>
-    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="75"/>
     </row>
-    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="75"/>
     </row>
-    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="75"/>
     </row>
-    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="75"/>
     </row>
-    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="75"/>
     </row>
-    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="75"/>
     </row>
   </sheetData>

</xml_diff>